<commit_message>
gros changement code html et css
</commit_message>
<xml_diff>
--- a/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Desktop\Projet_4_ Openclassroom\Projet-N-4\DOC SEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C22AB5-6598-4526-B740-52F373CA0C65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6627BB77-39A7-488F-A37F-F517806E71D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Categorie</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Référence</t>
   </si>
   <si>
-    <t>(SEO ou accessiblité ?)</t>
-  </si>
-  <si>
     <t>ces balises indiquent aux moteurs de recherche de quoi traite la page. Elles sont aussi affichées dans les résultats. Elles doivent donc non seulement contenir le mot-clé visé, mais aussi donner envie au visiteur de cliquer pour lire votre page.</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>taille des paragraphes</t>
   </si>
   <si>
-    <t>mettre la taille des textes d'une valeurs équivalent ou plus de 1em;</t>
-  </si>
-  <si>
     <t>mauvais nom de lien = &lt;page2</t>
   </si>
   <si>
@@ -88,9 +82,6 @@
     <t>changer le nom de "&lt;page2" par un nom plus approprié</t>
   </si>
   <si>
-    <t>présent sur les deux pages en haut à droite, Ligne 64 dans le code HTML,</t>
-  </si>
-  <si>
     <t>ne pas répéter par exemple le "contact"</t>
   </si>
   <si>
@@ -124,9 +115,6 @@
     <t>responsive /paragraphe beaucoup trop large</t>
   </si>
   <si>
-    <t>pour la page contact, le questionnaire est mal situé</t>
-  </si>
-  <si>
     <t>responsive / taille des images plus petites que les autres</t>
   </si>
   <si>
@@ -155,6 +143,48 @@
   </si>
   <si>
     <t>liste en trop en responsive sur la page contact ligne 57 du code HTML / logo mal fait : les deux pages en responsive ; ligne 970 dans le style,css</t>
+  </si>
+  <si>
+    <t>mettre la taille des textes d'une valeurs à ceux que ce soit plus visible pour les visiteurs</t>
+  </si>
+  <si>
+    <t>SEO ou accessibilité ?</t>
+  </si>
+  <si>
+    <t>l'adresse de la page plus intéressant de le mettre en page d'accueil</t>
+  </si>
+  <si>
+    <t>présent sur les deux pages en haut à droite, Ligne 64 dans le code HTML de la page d'accueil, Ligne 57 dans le code HTML de la page contact</t>
+  </si>
+  <si>
+    <t>Lorsque on insère des images par exemple dans un portefolio, il faut veiller à ce que les images soit de la meme taille</t>
+  </si>
+  <si>
+    <t>Si dans la page d'accueil les visiteurs sur téphone ou avec une page web réduite regarde les images avec deux de taille plus grande et deux autre avec des tailles plus petite, ca perd un coté éthestique, et les visiteurs ne sera pas tenté d'y preter attention</t>
+  </si>
+  <si>
+    <t>Mettre les 4 images avec des tailles identiques</t>
+  </si>
+  <si>
+    <t>Page d'accueil , les 4 images en milieu de page/ ligne 162 code HTML de la page d'accueil</t>
+  </si>
+  <si>
+    <t>Le questionnaire mal fait</t>
+  </si>
+  <si>
+    <t>Faire en sorte par exemple lors de la création d'un questionnaire de faire en sorte que les rectangles ou répondre aux questions posés soit plus agréable à regarder et qu'il ne fasse pas désordre quand on le regarde</t>
+  </si>
+  <si>
+    <t>Si le visiteur qui regarde le questionnaire voit les blocs de réponse mal agencé par et pas très esthétique ce la ne donnera pas forcément envie de répondre aux questions posés</t>
+  </si>
+  <si>
+    <t>Gérer les box de questionnement avec les flexbox serait plus pratique pour que ce soit plus agréable à regarder par exemple avec l'ajout d'un display : flex</t>
+  </si>
+  <si>
+    <t>Dans la page contact les blocs de questionnement /ligne 508 du code style.css</t>
+  </si>
+  <si>
+    <t>Le site est mal concu pour le responsive / pas de suivi google analytics ni de google seatch console moins bien référencé, le site n'est oas placé sur son nom de marque, acessible ou pas pour navigateur mobile et pour les personnes ayant un handicap, vitesse du site</t>
   </si>
 </sst>
 </file>
@@ -164,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -206,6 +236,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -221,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -264,15 +300,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed"/>
@@ -305,6 +375,24 @@
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
   </cellXfs>
@@ -522,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -540,346 +628,366 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7" t="s">
+    </row>
+    <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12" t="s">
+      <c r="C4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:26" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:26" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:26" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="78" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:26" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:26" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:26" ht="189.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="11"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1851,7 +1959,6 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
ajout de quelque recommandation + voir pour l'analyse du SEO
</commit_message>
<xml_diff>
--- a/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Desktop\Projet_4_ Openclassroom\Projet-N-4\DOC SEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6627BB77-39A7-488F-A37F-F517806E71D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077E0DC3-9503-463F-B20A-A79284492EC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Categorie</t>
   </si>
@@ -55,42 +55,15 @@
     <t>pour le titre voir l'URL et dans le code HTML ligne 31 et pour la description voir la ligne 6 du code HTML</t>
   </si>
   <si>
-    <t>taille des paragraphes</t>
-  </si>
-  <si>
-    <t>mauvais nom de lien = &lt;page2</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>mettre un nom de lien qui décrit bien le nom de la page en question</t>
-  </si>
-  <si>
-    <t>Si la taille des paragraphes est trop petite, sa n'attitrera pas les visiteurs à regarder le texte</t>
-  </si>
-  <si>
-    <t>Mettre les paragraphes plus gros pour amélioré la lisibilité</t>
-  </si>
-  <si>
-    <t>Tous les sous-texte dans la page d'accueil et l'adresse de l'agence dans la 2 ème page</t>
-  </si>
-  <si>
-    <t>peut induire en erreur le visiteur avec la syntaxe du mot qui n'est pas correcte</t>
-  </si>
-  <si>
-    <t>changer le nom de "&lt;page2" par un nom plus approprié</t>
-  </si>
-  <si>
     <t>ne pas répéter par exemple le "contact"</t>
   </si>
   <si>
     <t>&lt;meta "keyword"&gt; ?</t>
   </si>
   <si>
-    <t>Utilisation d'image à la place de par exemple de balise &lt;p&gt; ou &lt;h2&gt;</t>
-  </si>
-  <si>
     <t>ajout de contenu suplémentaire pas nécessaire</t>
   </si>
   <si>
@@ -100,21 +73,6 @@
     <t xml:space="preserve">enlever le "toggle navigation" présent sur la deuxième page et les liens ramenant sur le meme site ne sont pas utiles et enfin supprimer le rajout d'une div contenant des mots clés </t>
   </si>
   <si>
-    <t>Ne pas utiliser d'image pour y inclure du texte, il faut utiliser des balises type "block" en fonction de l'importance du texte</t>
-  </si>
-  <si>
-    <t>retaper l'entiéreté du texte dans des balises &lt;p&gt; ou &lt;h2&gt;</t>
-  </si>
-  <si>
-    <t>page d'accueil / ligne 96 + 136 + 166 du code HTML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si on utilise des images pour y importer google ne reconnaitra pas l'importance du texte alors qu'en y mettant des balises adapté google reconnaitra l'importance du texte  </t>
-  </si>
-  <si>
-    <t>responsive /paragraphe beaucoup trop large</t>
-  </si>
-  <si>
     <t>responsive / taille des images plus petites que les autres</t>
   </si>
   <si>
@@ -145,18 +103,12 @@
     <t>liste en trop en responsive sur la page contact ligne 57 du code HTML / logo mal fait : les deux pages en responsive ; ligne 970 dans le style,css</t>
   </si>
   <si>
-    <t>mettre la taille des textes d'une valeurs à ceux que ce soit plus visible pour les visiteurs</t>
-  </si>
-  <si>
     <t>SEO ou accessibilité ?</t>
   </si>
   <si>
     <t>l'adresse de la page plus intéressant de le mettre en page d'accueil</t>
   </si>
   <si>
-    <t>présent sur les deux pages en haut à droite, Ligne 64 dans le code HTML de la page d'accueil, Ligne 57 dans le code HTML de la page contact</t>
-  </si>
-  <si>
     <t>Lorsque on insère des images par exemple dans un portefolio, il faut veiller à ce que les images soit de la meme taille</t>
   </si>
   <si>
@@ -185,6 +137,9 @@
   </si>
   <si>
     <t>Le site est mal concu pour le responsive / pas de suivi google analytics ni de google seatch console moins bien référencé, le site n'est oas placé sur son nom de marque, acessible ou pas pour navigateur mobile et pour les personnes ayant un handicap, vitesse du site</t>
+  </si>
+  <si>
+    <t>Pas de suivi Google analytics</t>
   </si>
 </sst>
 </file>
@@ -194,7 +149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -239,6 +194,13 @@
     <font>
       <sz val="12"/>
       <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -341,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -393,6 +355,9 @@
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
   </cellXfs>
@@ -610,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -669,7 +634,7 @@
     </row>
     <row r="2" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
@@ -695,191 +660,161 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
-      <c r="B4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="B4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:26" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="D6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F6" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:26" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
-      <c r="B10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="8"/>
+      <c r="B10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:26" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
+    <row r="11" spans="1:26" ht="189.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="B11" s="11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
-      <c r="B12" s="11" t="s">
-        <v>32</v>
+      <c r="B12" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
-      <c r="B13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
-      <c r="B14" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:26" ht="189.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>53</v>
-      </c>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -894,7 +829,7 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -902,7 +837,7 @@
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -910,85 +845,57 @@
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1955,10 +1862,6 @@
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
commcement pour l'accesibilité  continué la syntaxe des réponses pour les livrables
</commit_message>
<xml_diff>
--- a/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Desktop\Projet_4_ Openclassroom\Projet-N-4\DOC SEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077E0DC3-9503-463F-B20A-A79284492EC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AD435E-22F3-4ACF-8ADE-6FA0A0B57272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Categorie</t>
   </si>
@@ -55,60 +55,9 @@
     <t>pour le titre voir l'URL et dans le code HTML ligne 31 et pour la description voir la ligne 6 du code HTML</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>ne pas répéter par exemple le "contact"</t>
-  </si>
-  <si>
-    <t>&lt;meta "keyword"&gt; ?</t>
-  </si>
-  <si>
-    <t>ajout de contenu suplémentaire pas nécessaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ne pas ajouter du contenu supplémentaire qui n'est pas utile pour le site </t>
-  </si>
-  <si>
-    <t xml:space="preserve">enlever le "toggle navigation" présent sur la deuxième page et les liens ramenant sur le meme site ne sont pas utiles et enfin supprimer le rajout d'une div contenant des mots clés </t>
-  </si>
-  <si>
-    <t>responsive / taille des images plus petites que les autres</t>
-  </si>
-  <si>
-    <t>reponsive/ ajout d'une puce en trop à la page contact + logo mal fait + liste des partenaires beaucoup trop longue</t>
-  </si>
-  <si>
-    <t>Element caché ou invisible</t>
-  </si>
-  <si>
-    <t>Ajouter du contenu supplémentaire qui est inutile n'est pas bon pour le SEO et les visiteurs ne seront pas attirés avec un contenu qui se voit surchagé et inutile,</t>
-  </si>
-  <si>
-    <t>Le fait de rajouter des mots-clés cachés et de le répéter sans cesse dans votre page s'appelle du "keyword stuffing" et est une technique Black Hat. Qui en gros si google le décide peut etre amener à vous bloquer votre site web</t>
-  </si>
-  <si>
-    <t>Ne pas rajouter des div contenant les mots-clés en les dissimulant sur le site</t>
-  </si>
-  <si>
-    <t>les deux lignes qui entourent le logo sont en faite un texte caché écrit en 1 px/ ligne 49 et 51 du code HTML de la page d'accueil et tout en bas il y a texte invisible qui contient aussi les mots-clés cachés présent sur la ligne 256 du code HTML de la page d'accueil</t>
-  </si>
-  <si>
-    <t>Rajouter simplement dans la balise head votre div avec vos mots-clés, et ne pas en rajouter.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toggle navigation = 2ème page/  liens en supplément = page d'accueil, page contact ligne 56 code HTML page d'accueil /div avec les mots-clés = page d'accueil / </t>
-  </si>
-  <si>
-    <t>liste en trop en responsive sur la page contact ligne 57 du code HTML / logo mal fait : les deux pages en responsive ; ligne 970 dans le style,css</t>
-  </si>
-  <si>
     <t>SEO ou accessibilité ?</t>
   </si>
   <si>
-    <t>l'adresse de la page plus intéressant de le mettre en page d'accueil</t>
-  </si>
-  <si>
     <t>Lorsque on insère des images par exemple dans un portefolio, il faut veiller à ce que les images soit de la meme taille</t>
   </si>
   <si>
@@ -121,25 +70,86 @@
     <t>Page d'accueil , les 4 images en milieu de page/ ligne 162 code HTML de la page d'accueil</t>
   </si>
   <si>
-    <t>Le questionnaire mal fait</t>
-  </si>
-  <si>
-    <t>Faire en sorte par exemple lors de la création d'un questionnaire de faire en sorte que les rectangles ou répondre aux questions posés soit plus agréable à regarder et qu'il ne fasse pas désordre quand on le regarde</t>
-  </si>
-  <si>
-    <t>Si le visiteur qui regarde le questionnaire voit les blocs de réponse mal agencé par et pas très esthétique ce la ne donnera pas forcément envie de répondre aux questions posés</t>
-  </si>
-  <si>
-    <t>Gérer les box de questionnement avec les flexbox serait plus pratique pour que ce soit plus agréable à regarder par exemple avec l'ajout d'un display : flex</t>
-  </si>
-  <si>
-    <t>Dans la page contact les blocs de questionnement /ligne 508 du code style.css</t>
-  </si>
-  <si>
-    <t>Le site est mal concu pour le responsive / pas de suivi google analytics ni de google seatch console moins bien référencé, le site n'est oas placé sur son nom de marque, acessible ou pas pour navigateur mobile et pour les personnes ayant un handicap, vitesse du site</t>
-  </si>
-  <si>
     <t>Pas de suivi Google analytics</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>balise &lt;meta "keyword"&gt;</t>
+  </si>
+  <si>
+    <t>mettre le contenu de la balise en question dans la balise &lt;head&gt; du code HTML avec des mots-clés qui concorde avec le thème du site, Les mots-clés doivent apparaitre au moins une fois dans le titre &lt;h1&gt;</t>
+  </si>
+  <si>
+    <t>Ne placer la balise &lt;meta name="keywords" content="" dans le &lt;head&gt; du code HTML et non pas dans le body, Et viser des mots-clés plus en accord avec votre site,</t>
+  </si>
+  <si>
+    <t>Si les mots-clés sont mal intégrés dans le code HTML, ou, on un contenu qui n'est pas logique par rapport à la thématique du site. Ceci ne sera pas bon pour le SEO et si est caché sur la page web, il sera considéré comme du contenu black hat.</t>
+  </si>
+  <si>
+    <t>ligne 5 du code HTML / et présence de contenu duplicatif de la balise keyword sur la page d'accueil</t>
+  </si>
+  <si>
+    <t>Le site n'est pas placé sur son nom de marque</t>
+  </si>
+  <si>
+    <t>Vitesse de chargement du site trop longue</t>
+  </si>
+  <si>
+    <t>pas de fichier robot.txt</t>
+  </si>
+  <si>
+    <t>problème d'indexation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acessible ou pas pour navigateur mobile et pour les personnes ayant un handicap. 
+</t>
+  </si>
+  <si>
+    <t>responsive / taille des images plus petites que les autres + ((liste des partenaires trop longue))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> s'inscrire ou se connecter à Google Analytics et renseigner l'URL de votre site. Vous pourrez ensuite récupérer le code de suivi qu'il faudra copier puis coller entre les balises&lt;head&gt;&lt;/head&gt;de toutes vos pages HTML.</t>
+  </si>
+  <si>
+    <t>Si il n'y à pas de suivi google analytics, vous ne pourrez pas vous rendre compte du nombre de visiteur qui viennent sur votre site. Et vous pourrez par la suite étudier également le comportement de vos visiteur si des pages sont plus visités que d'autre ou si un jour ou l'autre vous avez une perte de trafic.</t>
+  </si>
+  <si>
+    <t>Il est donc recommander un code de suivi lié à l'URL de votre site dans les balise &lt;head&gt; de toutes vos pages web. Et de regarde quotidiennement le rendement de vos visteurs sur Google analytics</t>
+  </si>
+  <si>
+    <t>code HTML des 2 pages web</t>
+  </si>
+  <si>
+    <t>Avoir un suivi avec google search console, notamment en y intégrant un sitemap</t>
+  </si>
+  <si>
+    <t>Le fait d'avoir un suivi avec la search console vous permet d'avoir des informations très précises sur ce que vos visiteurs recherchent sur Google pour vous trouver. Et le fait de mettre en place un sitemap permet d'avoir un plan du site contenant toutes les pages de votre site qui doivent être indexées.</t>
+  </si>
+  <si>
+    <t>Pas de suivi avec la google search console</t>
+  </si>
+  <si>
+    <t>renseigner son URL dans la search console, puis y rajouter un sitemap</t>
+  </si>
+  <si>
+    <t>Aucun sitemap présent dans les dossiers du site</t>
+  </si>
+  <si>
+    <t>Faite en sorte que la vitesse du site ne soit pas trop longue en regardant par exemple les erreurs qui font ralentir votre sitre sur gtmetrix.com</t>
+  </si>
+  <si>
+    <t>en regardant le résulat donné par le site gtmetrix.com qui examine les perfomances de votre site</t>
+  </si>
+  <si>
+    <t>Si la vitesse de chargement est trop longue, cela impactera énormément sur vos visiteurs car si la page est trop longue à charger, le visiteur n'aura pas forcément l'envie d'attendre que la page se charge.</t>
+  </si>
+  <si>
+    <t>toujours vérifier avec gtmetrix.com ou d'autre outil que votre page est bien optimisé. Pour éviter ce problème optimiser vos images, minifier et compresser vos ressources CSS et JS et débloquer le téléchargement de vos pages</t>
+  </si>
+  <si>
+    <t>VOIR SITEMPA</t>
   </si>
 </sst>
 </file>
@@ -149,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,22 +195,14 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="4"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="9" tint="-0.249977111117893"/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -219,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -244,19 +246,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -303,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -327,16 +316,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -345,19 +328,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
   </cellXfs>
@@ -575,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -593,22 +585,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1"/>
@@ -633,18 +625,20 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
+      <c r="A2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -660,238 +654,201 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="129" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="D5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+    <row r="6" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="8" t="s">
+    <row r="7" spans="1:26" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18"/>
+      <c r="B7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:26" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
-    <row r="7" spans="1:26" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="8" t="s">
+    <row r="12" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="B12" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" ht="189.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1855,13 +1812,6 @@
     <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
changemnt couleur pour contraste
</commit_message>
<xml_diff>
--- a/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Desktop\Projet_4_ Openclassroom\Projet-N-4\DOC SEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AD435E-22F3-4ACF-8ADE-6FA0A0B57272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE52FC8-59B1-4468-B14C-529C1BDC8114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Categorie</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>VOIR SITEMPA</t>
+  </si>
+  <si>
+    <t>Le contraste des couleurs</t>
+  </si>
+  <si>
+    <t>Acessibilité</t>
+  </si>
+  <si>
+    <t>les images et leur texte alternatif</t>
   </si>
 </sst>
 </file>
@@ -569,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -794,17 +803,25 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+    <row r="13" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+    <row r="14" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>

</xml_diff>

<commit_message>
création des fichiers js minifier
</commit_message>
<xml_diff>
--- a/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Desktop\Projet_4_ Openclassroom\Projet-N-4\DOC SEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE52FC8-59B1-4468-B14C-529C1BDC8114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDDD4CC-F9FD-44EF-BEFD-69877F0C2C56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Categorie</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Ne placer la balise &lt;meta name="keywords" content="" dans le &lt;head&gt; du code HTML et non pas dans le body, Et viser des mots-clés plus en accord avec votre site,</t>
   </si>
   <si>
-    <t>Si les mots-clés sont mal intégrés dans le code HTML, ou, on un contenu qui n'est pas logique par rapport à la thématique du site. Ceci ne sera pas bon pour le SEO et si est caché sur la page web, il sera considéré comme du contenu black hat.</t>
-  </si>
-  <si>
     <t>ligne 5 du code HTML / et présence de contenu duplicatif de la balise keyword sur la page d'accueil</t>
   </si>
   <si>
@@ -103,62 +100,83 @@
     <t>problème d'indexation</t>
   </si>
   <si>
-    <t xml:space="preserve">acessible ou pas pour navigateur mobile et pour les personnes ayant un handicap. 
+    <t>responsive / taille des images plus petites que les autres + ((liste des partenaires trop longue))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> s'inscrire ou se connecter à Google Analytics et renseigner l'URL de votre site. Vous pourrez ensuite récupérer le code de suivi qu'il faudra copier puis coller entre les balises&lt;head&gt;&lt;/head&gt;de toutes vos pages HTML.</t>
+  </si>
+  <si>
+    <t>Si il n'y à pas de suivi google analytics, vous ne pourrez pas vous rendre compte du nombre de visiteur qui viennent sur votre site. Et vous pourrez par la suite étudier également le comportement de vos visiteur si des pages sont plus visités que d'autre ou si un jour ou l'autre vous avez une perte de trafic.</t>
+  </si>
+  <si>
+    <t>Il est donc recommander un code de suivi lié à l'URL de votre site dans les balise &lt;head&gt; de toutes vos pages web. Et de regarde quotidiennement le rendement de vos visteurs sur Google analytics</t>
+  </si>
+  <si>
+    <t>code HTML des 2 pages web</t>
+  </si>
+  <si>
+    <t>Avoir un suivi avec google search console, notamment en y intégrant un sitemap</t>
+  </si>
+  <si>
+    <t>Le fait d'avoir un suivi avec la search console vous permet d'avoir des informations très précises sur ce que vos visiteurs recherchent sur Google pour vous trouver. Et le fait de mettre en place un sitemap permet d'avoir un plan du site contenant toutes les pages de votre site qui doivent être indexées.</t>
+  </si>
+  <si>
+    <t>Pas de suivi avec la google search console</t>
+  </si>
+  <si>
+    <t>renseigner son URL dans la search console, puis y rajouter un sitemap</t>
+  </si>
+  <si>
+    <t>Aucun sitemap présent dans les dossiers du site</t>
+  </si>
+  <si>
+    <t>Faite en sorte que la vitesse du site ne soit pas trop longue en regardant par exemple les erreurs qui font ralentir votre sitre sur gtmetrix.com</t>
+  </si>
+  <si>
+    <t>Si la vitesse de chargement est trop longue, cela impactera énormément sur vos visiteurs car si la page est trop longue à charger, le visiteur n'aura pas forcément l'envie d'attendre que la page se charge.</t>
+  </si>
+  <si>
+    <t>toujours vérifier avec gtmetrix.com ou d'autre outil que votre page est bien optimisé. Pour éviter ce problème optimiser vos images, minifier et compresser vos ressources CSS et JS et débloquer le téléchargement de vos pages</t>
+  </si>
+  <si>
+    <t>VOIR SITEMPA</t>
+  </si>
+  <si>
+    <t>Le contraste des couleurs</t>
+  </si>
+  <si>
+    <t>Acessibilité</t>
+  </si>
+  <si>
+    <t>les images et leur texte alternatif</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>code HTML de la page d'accueil</t>
+  </si>
+  <si>
+    <t>Toujours au commencement de la création du site,mettre du contenu adéquat qui décrit votre site. Et ajouter le nom de votre marque ou un titre qui correspondrait au titre de votre site.</t>
+  </si>
+  <si>
+    <t>Dans la balise  &lt;title&gt; et description du code HTML de la page d'accueil mettre du contenu de qualité et cohérent.</t>
+  </si>
+  <si>
+    <t>Les balises &lt;title&gt; et &lt;description&gt;  indiquent aux moteurs de recherche de quoi traite la page. Elles sont aussi affichées dans les résultats. Elles doivent donc non seulement contenir le mot-clé visé, mais aussi donner envie au visiteur de cliquer pour lire votre page.</t>
+  </si>
+  <si>
+    <t>En regardant le résulat donné par le site gtmetrix.com qui examine les perfomances de votre site</t>
+  </si>
+  <si>
+    <t>ou plutôt manque d'accessibilité pour les personne ayant un handicap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accesible pour navigateur mobile
 </t>
   </si>
   <si>
-    <t>responsive / taille des images plus petites que les autres + ((liste des partenaires trop longue))</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> s'inscrire ou se connecter à Google Analytics et renseigner l'URL de votre site. Vous pourrez ensuite récupérer le code de suivi qu'il faudra copier puis coller entre les balises&lt;head&gt;&lt;/head&gt;de toutes vos pages HTML.</t>
-  </si>
-  <si>
-    <t>Si il n'y à pas de suivi google analytics, vous ne pourrez pas vous rendre compte du nombre de visiteur qui viennent sur votre site. Et vous pourrez par la suite étudier également le comportement de vos visiteur si des pages sont plus visités que d'autre ou si un jour ou l'autre vous avez une perte de trafic.</t>
-  </si>
-  <si>
-    <t>Il est donc recommander un code de suivi lié à l'URL de votre site dans les balise &lt;head&gt; de toutes vos pages web. Et de regarde quotidiennement le rendement de vos visteurs sur Google analytics</t>
-  </si>
-  <si>
-    <t>code HTML des 2 pages web</t>
-  </si>
-  <si>
-    <t>Avoir un suivi avec google search console, notamment en y intégrant un sitemap</t>
-  </si>
-  <si>
-    <t>Le fait d'avoir un suivi avec la search console vous permet d'avoir des informations très précises sur ce que vos visiteurs recherchent sur Google pour vous trouver. Et le fait de mettre en place un sitemap permet d'avoir un plan du site contenant toutes les pages de votre site qui doivent être indexées.</t>
-  </si>
-  <si>
-    <t>Pas de suivi avec la google search console</t>
-  </si>
-  <si>
-    <t>renseigner son URL dans la search console, puis y rajouter un sitemap</t>
-  </si>
-  <si>
-    <t>Aucun sitemap présent dans les dossiers du site</t>
-  </si>
-  <si>
-    <t>Faite en sorte que la vitesse du site ne soit pas trop longue en regardant par exemple les erreurs qui font ralentir votre sitre sur gtmetrix.com</t>
-  </si>
-  <si>
-    <t>en regardant le résulat donné par le site gtmetrix.com qui examine les perfomances de votre site</t>
-  </si>
-  <si>
-    <t>Si la vitesse de chargement est trop longue, cela impactera énormément sur vos visiteurs car si la page est trop longue à charger, le visiteur n'aura pas forcément l'envie d'attendre que la page se charge.</t>
-  </si>
-  <si>
-    <t>toujours vérifier avec gtmetrix.com ou d'autre outil que votre page est bien optimisé. Pour éviter ce problème optimiser vos images, minifier et compresser vos ressources CSS et JS et débloquer le téléchargement de vos pages</t>
-  </si>
-  <si>
-    <t>VOIR SITEMPA</t>
-  </si>
-  <si>
-    <t>Le contraste des couleurs</t>
-  </si>
-  <si>
-    <t>Acessibilité</t>
-  </si>
-  <si>
-    <t>les images et leur texte alternatif</t>
+    <t>Si les mots-clés sont mal intégrés dans le code HTML, ou, on un contenu qui n'est pas logique par rapport à la thématique du site, ceci ne sera pas bon pour le SEO. Et si des attribut "keywords" sont caché sur la page web, il sera considéré comme du contenu black hat.</t>
   </si>
 </sst>
 </file>
@@ -204,19 +222,21 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="4"/>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="14"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +247,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -301,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -349,17 +381,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -663,7 +701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>17</v>
       </c>
@@ -674,19 +712,19 @@
         <v>19</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="129" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
-        <v>28</v>
+      <c r="B5" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>12</v>
@@ -709,156 +747,161 @@
         <v>16</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="8" t="s">
+    </row>
+    <row r="7" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>32</v>
       </c>
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+    <row r="8" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="8" t="s">
+    <row r="9" spans="1:26" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>37</v>
       </c>
+      <c r="E9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>17</v>
-      </c>
+    <row r="10" spans="1:26" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9"/>
       <c r="B10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>39</v>
-      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+    <row r="12" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>45</v>
+    <row r="14" spans="1:26" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+      <c r="B15" s="22" t="s">
+        <v>50</v>
+      </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1828,7 +1871,6 @@
     <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
supprimation des annuaires + voir pour minifier le css
</commit_message>
<xml_diff>
--- a/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/DOC SEO/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Desktop\Projet_4_ Openclassroom\Projet-N-4\DOC SEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDDD4CC-F9FD-44EF-BEFD-69877F0C2C56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ACA091-0921-4143-8AEC-AE6549F5A4C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Categorie</t>
   </si>
@@ -97,9 +97,6 @@
     <t>pas de fichier robot.txt</t>
   </si>
   <si>
-    <t>problème d'indexation</t>
-  </si>
-  <si>
     <t>responsive / taille des images plus petites que les autres + ((liste des partenaires trop longue))</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>Le fait d'avoir un suivi avec la search console vous permet d'avoir des informations très précises sur ce que vos visiteurs recherchent sur Google pour vous trouver. Et le fait de mettre en place un sitemap permet d'avoir un plan du site contenant toutes les pages de votre site qui doivent être indexées.</t>
   </si>
   <si>
-    <t>Pas de suivi avec la google search console</t>
-  </si>
-  <si>
     <t>renseigner son URL dans la search console, puis y rajouter un sitemap</t>
   </si>
   <si>
@@ -139,9 +133,6 @@
     <t>toujours vérifier avec gtmetrix.com ou d'autre outil que votre page est bien optimisé. Pour éviter ce problème optimiser vos images, minifier et compresser vos ressources CSS et JS et débloquer le téléchargement de vos pages</t>
   </si>
   <si>
-    <t>VOIR SITEMPA</t>
-  </si>
-  <si>
     <t>Le contraste des couleurs</t>
   </si>
   <si>
@@ -172,11 +163,10 @@
     <t>ou plutôt manque d'accessibilité pour les personne ayant un handicap</t>
   </si>
   <si>
-    <t xml:space="preserve">accesible pour navigateur mobile
-</t>
-  </si>
-  <si>
     <t>Si les mots-clés sont mal intégrés dans le code HTML, ou, on un contenu qui n'est pas logique par rapport à la thématique du site, ceci ne sera pas bon pour le SEO. Et si des attribut "keywords" sont caché sur la page web, il sera considéré comme du contenu black hat.</t>
+  </si>
+  <si>
+    <t>présence d'un sitemap + sitemap dans la search console</t>
   </si>
 </sst>
 </file>
@@ -186,7 +176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -203,10 +193,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="12"/>
@@ -235,6 +221,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -257,7 +265,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -345,59 +353,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="distributed" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -632,22 +643,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1"/>
@@ -672,181 +683,177 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="129" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>44</v>
+      <c r="F8" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>48</v>
+      <c r="F9" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>40</v>
+      <c r="A12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>37</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -854,11 +861,11 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>41</v>
+      <c r="A13" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -866,9 +873,12 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="21" t="s">
-        <v>49</v>
+      <c r="A14" s="22" t="e">
+        <f>+A7AA3:A14</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>46</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -877,9 +887,7 @@
     </row>
     <row r="15" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="22" t="s">
-        <v>50</v>
-      </c>
+      <c r="B15" s="18"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>

</xml_diff>